<commit_message>
media url added to data. dataset: 0107T31122020
</commit_message>
<xml_diff>
--- a/btp-01122020T10012021.xlsx
+++ b/btp-01122020T10012021.xlsx
@@ -1,20 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mysor\Documents\Coding\traffic_tweet_analysis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CEE409C-C056-47F9-9755-F8D7A801E87F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="617">
   <si>
     <t>in_reply_to_user_id</t>
   </si>
@@ -1905,12 +1912,48 @@
   <si>
     <t>@vijayanagartrps @btppubliceye there's no No Parking on this side of the road next to ttmc Vijaynagar yet the bike towed away, don't understand how it works.. https://t.co/O4CU0Mz7jd</t>
   </si>
+  <si>
+    <t>PoliceViolation</t>
+  </si>
+  <si>
+    <t>PublicNuisance</t>
+  </si>
+  <si>
+    <t>SignalNW</t>
+  </si>
+  <si>
+    <t>Unspecified</t>
+  </si>
+  <si>
+    <t>ParkingViolation</t>
+  </si>
+  <si>
+    <t>Clarification</t>
+  </si>
+  <si>
+    <t>FaultyNumberPlate</t>
+  </si>
+  <si>
+    <t>PublicWork</t>
+  </si>
+  <si>
+    <t>StuntDriving</t>
+  </si>
+  <si>
+    <t>RidingViolation</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>TrafficJam</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1950,9 +1993,7 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -1962,18 +2003,99 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C70FFD2-25A5-471D-A64E-8922DDA40A5C}" name="Table1" displayName="Table1" ref="A1:H111" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
+  <autoFilter ref="A1:H111" xr:uid="{E1A3123D-7194-423F-A6E9-6F56519A2A07}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{8899A7A2-0F60-4295-8FB7-A7A95A7A5FF1}" name="in_reply_to_user_id"/>
+    <tableColumn id="2" xr3:uid="{2FA710F6-D0F9-44B6-8F90-7E1039D326CD}" name="text" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{299DD635-95F6-4B3B-8C9B-8C1D374C0DB0}" name="original_tweet" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{933431C5-B15F-4898-9192-E422D6FAC3A6}" name="created_at"/>
+    <tableColumn id="4" xr3:uid="{F669A14C-858F-4D32-B6BD-7B5C7C45AD43}" name="id"/>
+    <tableColumn id="5" xr3:uid="{7522233D-4539-4FBB-9197-FAFDAA3EDD9D}" name="referenced_tweets"/>
+    <tableColumn id="6" xr3:uid="{BCF0E73C-8264-4299-B4C4-5EAC7F416DF6}" name="attachments.media_keys"/>
+    <tableColumn id="8" xr3:uid="{0275B830-DEEC-46C4-A13F-8282E94125C2}" name="Label"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2019,7 +2141,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2051,9 +2173,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2085,6 +2225,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2260,2201 +2418,2419 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G111"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="H79" sqref="H79"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.5546875" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" customWidth="1"/>
+    <col min="3" max="3" width="49.21875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" customWidth="1"/>
+    <col min="7" max="7" width="24" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="D2" t="s">
         <v>179</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>289</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>399</v>
       </c>
-      <c r="G2" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="D3" t="s">
         <v>180</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>290</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>400</v>
       </c>
-      <c r="G3" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="D4" t="s">
         <v>181</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>291</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>401</v>
       </c>
-      <c r="G4" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="D5" t="s">
         <v>182</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>292</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>402</v>
       </c>
-      <c r="G5" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="D6" t="s">
         <v>183</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>293</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>403</v>
       </c>
-      <c r="G6" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="D7" t="s">
         <v>184</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>294</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>404</v>
       </c>
-      <c r="G7" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="D8" t="s">
         <v>185</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>295</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>405</v>
       </c>
-      <c r="G8" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="D9" t="s">
         <v>186</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>296</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>406</v>
       </c>
-      <c r="G9" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="D10" t="s">
         <v>187</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>297</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>407</v>
       </c>
-      <c r="G10" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="D11" t="s">
         <v>188</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>298</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>408</v>
       </c>
-      <c r="G11" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="D12" t="s">
         <v>189</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>299</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>409</v>
       </c>
-      <c r="G12" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="D13" t="s">
         <v>190</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>300</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>410</v>
       </c>
-      <c r="G13" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="D14" t="s">
         <v>191</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>301</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>411</v>
       </c>
-      <c r="G14" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="D15" t="s">
         <v>192</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>302</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>412</v>
       </c>
-      <c r="G15" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H15" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="D16" t="s">
         <v>193</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>303</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>413</v>
       </c>
-      <c r="G16" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="D17" t="s">
         <v>194</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>304</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>414</v>
       </c>
-      <c r="G17" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="D18" t="s">
         <v>195</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>305</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>415</v>
       </c>
-      <c r="G18" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="D19" t="s">
         <v>196</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>306</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>416</v>
       </c>
-      <c r="G19" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="H19" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="D20" t="s">
         <v>197</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>307</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>417</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>507</v>
       </c>
-      <c r="G20" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="D21" t="s">
         <v>198</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>308</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>418</v>
       </c>
-      <c r="G21" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H21" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="D22" t="s">
         <v>199</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>309</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>419</v>
       </c>
-      <c r="G22" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>16</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="D23" t="s">
         <v>200</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>310</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>411</v>
       </c>
-      <c r="G23" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>17</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="D24" t="s">
         <v>201</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>311</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>412</v>
       </c>
-      <c r="G24" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>12</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="D25" t="s">
         <v>202</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>312</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>420</v>
       </c>
-      <c r="G25" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="H25" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>23</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="D26" t="s">
         <v>203</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>313</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>421</v>
       </c>
-      <c r="G26" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>14</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="D27" t="s">
         <v>204</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>314</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>422</v>
       </c>
-      <c r="G27" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>24</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="D28" t="s">
         <v>205</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>315</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>423</v>
       </c>
-      <c r="G28" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="H28" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>25</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="D29" t="s">
         <v>206</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>316</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>424</v>
       </c>
-      <c r="G29" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="H29" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>26</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="D30" t="s">
         <v>207</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>317</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>425</v>
       </c>
-      <c r="G30" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="H30" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>27</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="D31" t="s">
         <v>208</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>318</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>426</v>
       </c>
-      <c r="G31" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="H31" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>28</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="D32" t="s">
         <v>209</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>319</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>427</v>
       </c>
-      <c r="G32" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>29</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="D33" t="s">
         <v>210</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>320</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>428</v>
       </c>
-      <c r="G33" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>30</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="D34" t="s">
         <v>211</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>321</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>429</v>
       </c>
-      <c r="G34" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="H34" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>31</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="D35" t="s">
         <v>212</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>322</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>430</v>
       </c>
-      <c r="G35" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="H35" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>14</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="D36" t="s">
         <v>213</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>323</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>431</v>
       </c>
-      <c r="G36" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="H36" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>14</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="D37" t="s">
         <v>214</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>324</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>432</v>
       </c>
-      <c r="G37" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="B38" t="s">
+      <c r="H37" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B38" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="D38" t="s">
         <v>215</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>325</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>433</v>
       </c>
-      <c r="G38" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+    </row>
+    <row r="39" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>32</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="D39" t="s">
         <v>216</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>326</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>434</v>
       </c>
-      <c r="G39" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+    </row>
+    <row r="40" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>12</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>217</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>327</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>33</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="D41" t="s">
         <v>218</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>328</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>436</v>
       </c>
-      <c r="G41" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
+    </row>
+    <row r="42" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>11</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="D42" t="s">
         <v>219</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>329</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>437</v>
       </c>
-      <c r="G42" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
+      <c r="H42" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>13</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="D43" t="s">
         <v>220</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>330</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>438</v>
       </c>
-      <c r="G43" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+      <c r="H43" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>34</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="D44" t="s">
         <v>221</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>331</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
         <v>439</v>
       </c>
-      <c r="G44" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+    </row>
+    <row r="45" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>33</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="D45" t="s">
         <v>222</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>332</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>440</v>
       </c>
-      <c r="G45" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="H45" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>35</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="D46" t="s">
         <v>223</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>333</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>441</v>
       </c>
-      <c r="G46" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+      <c r="H46" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>36</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="D47" t="s">
         <v>224</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>334</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>442</v>
       </c>
-      <c r="G47" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+      <c r="H47" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>37</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="D48" t="s">
         <v>225</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>335</v>
       </c>
-      <c r="E48" t="s">
+      <c r="F48" t="s">
         <v>443</v>
       </c>
-      <c r="G48" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
+      <c r="H48" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>38</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="D49" t="s">
         <v>226</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>336</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>444</v>
       </c>
-      <c r="G49" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
+      <c r="H49" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>39</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="D50" t="s">
         <v>227</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>337</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>445</v>
       </c>
-      <c r="G50" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
+      <c r="H50" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>40</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="D51" t="s">
         <v>228</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>338</v>
       </c>
-      <c r="E51" t="s">
+      <c r="F51" t="s">
         <v>446</v>
       </c>
-      <c r="G51" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
+      <c r="H51" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>41</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="D52" t="s">
         <v>229</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>339</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
         <v>447</v>
       </c>
-      <c r="G52" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
+      <c r="H52" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>39</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>230</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>340</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>42</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="D54" t="s">
         <v>231</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>341</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>449</v>
       </c>
-      <c r="F54" t="s">
+      <c r="G54" t="s">
         <v>508</v>
       </c>
-      <c r="G54" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
+      <c r="H54" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>20</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="D55" t="s">
         <v>232</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>342</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F55" t="s">
         <v>450</v>
       </c>
-      <c r="G55" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
+      <c r="H55" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>43</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="D56" t="s">
         <v>233</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>343</v>
       </c>
-      <c r="E56" t="s">
+      <c r="F56" t="s">
         <v>451</v>
       </c>
-      <c r="G56" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
+      <c r="H56" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>44</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>234</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>344</v>
       </c>
-      <c r="E57" t="s">
+      <c r="F57" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>45</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="D58" t="s">
         <v>235</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>345</v>
       </c>
-      <c r="E58" t="s">
+      <c r="F58" t="s">
         <v>453</v>
       </c>
-      <c r="G58" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
+      <c r="H58" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>30</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>236</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>346</v>
       </c>
-      <c r="E59" t="s">
+      <c r="F59" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>7</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="D60" t="s">
         <v>237</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>347</v>
       </c>
-      <c r="E60" t="s">
+      <c r="F60" t="s">
         <v>455</v>
       </c>
-      <c r="G60" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
+      <c r="H60" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>30</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="D61" t="s">
         <v>238</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>348</v>
       </c>
-      <c r="E61" t="s">
+      <c r="F61" t="s">
         <v>456</v>
       </c>
-      <c r="G61" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
+    </row>
+    <row r="62" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>46</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="D62" t="s">
         <v>239</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>349</v>
       </c>
-      <c r="E62" t="s">
+      <c r="F62" t="s">
         <v>457</v>
       </c>
-      <c r="G62" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
+    </row>
+    <row r="63" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>7</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="D63" t="s">
         <v>240</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>350</v>
       </c>
-      <c r="E63" t="s">
+      <c r="F63" t="s">
         <v>458</v>
       </c>
-      <c r="G63" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
+      <c r="H63" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>47</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="D64" t="s">
         <v>241</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>351</v>
       </c>
-      <c r="E64" t="s">
+      <c r="F64" t="s">
         <v>459</v>
       </c>
-      <c r="G64" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
+      <c r="H64" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>48</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="D65" t="s">
         <v>242</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>352</v>
       </c>
-      <c r="E65" t="s">
+      <c r="F65" t="s">
         <v>460</v>
       </c>
-      <c r="G65" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
+    </row>
+    <row r="66" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>48</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="D66" t="s">
         <v>243</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>353</v>
       </c>
-      <c r="E66" t="s">
+      <c r="F66" t="s">
         <v>461</v>
       </c>
-      <c r="G66" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
+      <c r="H66" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>49</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="D67" t="s">
         <v>244</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>354</v>
       </c>
-      <c r="E67" t="s">
+      <c r="F67" t="s">
         <v>462</v>
       </c>
-      <c r="G67" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
+      <c r="H67" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>50</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D68" t="s">
         <v>245</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>355</v>
       </c>
-      <c r="E68" t="s">
+      <c r="F68" t="s">
         <v>463</v>
       </c>
-      <c r="G68" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
+      <c r="H68" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>50</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="D69" t="s">
         <v>246</v>
       </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
         <v>356</v>
       </c>
-      <c r="E69" t="s">
+      <c r="F69" t="s">
         <v>464</v>
       </c>
-      <c r="G69" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7">
+      <c r="H69" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>30</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>247</v>
       </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
         <v>357</v>
       </c>
-      <c r="E70" t="s">
+      <c r="F70" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>51</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="D71" t="s">
         <v>248</v>
       </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
         <v>358</v>
       </c>
-      <c r="E71" t="s">
+      <c r="F71" t="s">
         <v>466</v>
       </c>
-      <c r="G71" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7">
+      <c r="H71" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>30</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C72" t="s">
+      <c r="D72" t="s">
         <v>249</v>
       </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
         <v>359</v>
       </c>
-      <c r="E72" t="s">
+      <c r="F72" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>52</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="D73" t="s">
         <v>250</v>
       </c>
-      <c r="D73" t="s">
+      <c r="E73" t="s">
         <v>360</v>
       </c>
-      <c r="E73" t="s">
+      <c r="F73" t="s">
         <v>468</v>
       </c>
-      <c r="G73" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7">
+      <c r="H73" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>53</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="D74" t="s">
         <v>251</v>
       </c>
-      <c r="D74" t="s">
+      <c r="E74" t="s">
         <v>361</v>
       </c>
-      <c r="E74" t="s">
+      <c r="F74" t="s">
         <v>469</v>
       </c>
-      <c r="G74" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7">
+      <c r="H74" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>54</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="D75" t="s">
         <v>252</v>
       </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>362</v>
       </c>
-      <c r="E75" t="s">
+      <c r="F75" t="s">
         <v>470</v>
       </c>
-      <c r="G75" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7">
+      <c r="H75" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>49</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="D76" t="s">
         <v>253</v>
       </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
         <v>363</v>
       </c>
-      <c r="E76" t="s">
+      <c r="F76" t="s">
         <v>471</v>
       </c>
-      <c r="G76" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7">
+      <c r="H76" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>55</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="3" t="s">
+        <v>576</v>
+      </c>
+      <c r="D77" t="s">
         <v>254</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>364</v>
       </c>
-      <c r="E77" t="s">
+      <c r="F77" t="s">
         <v>472</v>
       </c>
-      <c r="G77" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
+    </row>
+    <row r="78" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>56</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="3" t="s">
+        <v>577</v>
+      </c>
+      <c r="D78" t="s">
         <v>255</v>
       </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
         <v>365</v>
       </c>
-      <c r="E78" t="s">
+      <c r="F78" t="s">
         <v>473</v>
       </c>
-      <c r="G78" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
+      <c r="H78" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>49</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="D79" t="s">
         <v>256</v>
       </c>
-      <c r="D79" t="s">
+      <c r="E79" t="s">
         <v>366</v>
       </c>
-      <c r="E79" t="s">
+      <c r="F79" t="s">
         <v>474</v>
       </c>
-      <c r="G79" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7">
+    </row>
+    <row r="80" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>57</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="D80" t="s">
         <v>257</v>
       </c>
-      <c r="D80" t="s">
+      <c r="E80" t="s">
         <v>367</v>
       </c>
-      <c r="E80" t="s">
+      <c r="F80" t="s">
         <v>475</v>
       </c>
-      <c r="G80" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7">
+    </row>
+    <row r="81" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>58</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="D81" t="s">
         <v>258</v>
       </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
         <v>368</v>
       </c>
-      <c r="E81" t="s">
+      <c r="F81" t="s">
         <v>476</v>
       </c>
-      <c r="G81" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7">
+    </row>
+    <row r="82" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>59</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="D82" t="s">
         <v>259</v>
       </c>
-      <c r="D82" t="s">
+      <c r="E82" t="s">
         <v>369</v>
       </c>
-      <c r="E82" t="s">
+      <c r="F82" t="s">
         <v>477</v>
       </c>
-      <c r="G82" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7">
+    </row>
+    <row r="83" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>60</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="D83" t="s">
         <v>260</v>
       </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>370</v>
       </c>
-      <c r="E83" t="s">
+      <c r="F83" t="s">
         <v>478</v>
       </c>
-      <c r="G83" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7">
+    </row>
+    <row r="84" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>61</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="D84" t="s">
         <v>261</v>
       </c>
-      <c r="D84" t="s">
+      <c r="E84" t="s">
         <v>371</v>
       </c>
-      <c r="E84" t="s">
+      <c r="F84" t="s">
         <v>479</v>
       </c>
-      <c r="G84" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7">
+    </row>
+    <row r="85" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>62</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="D85" t="s">
         <v>262</v>
       </c>
-      <c r="D85" t="s">
+      <c r="E85" t="s">
         <v>372</v>
       </c>
-      <c r="E85" t="s">
+      <c r="F85" t="s">
         <v>480</v>
       </c>
-      <c r="G85" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7">
+    </row>
+    <row r="86" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>30</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
         <v>263</v>
       </c>
-      <c r="D86" t="s">
+      <c r="E86" t="s">
         <v>373</v>
       </c>
-      <c r="E86" t="s">
+      <c r="F86" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>63</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="D87" t="s">
         <v>264</v>
       </c>
-      <c r="D87" t="s">
+      <c r="E87" t="s">
         <v>374</v>
       </c>
-      <c r="E87" t="s">
+      <c r="F87" t="s">
         <v>482</v>
       </c>
-      <c r="G87" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7">
+    </row>
+    <row r="88" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>31</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="D88" t="s">
         <v>265</v>
       </c>
-      <c r="D88" t="s">
+      <c r="E88" t="s">
         <v>375</v>
       </c>
-      <c r="E88" t="s">
+      <c r="F88" t="s">
         <v>483</v>
       </c>
-      <c r="G88" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7">
+    </row>
+    <row r="89" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>64</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="D89" t="s">
         <v>266</v>
       </c>
-      <c r="D89" t="s">
+      <c r="E89" t="s">
         <v>376</v>
       </c>
-      <c r="E89" t="s">
+      <c r="F89" t="s">
         <v>484</v>
       </c>
-      <c r="G89" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7">
+    </row>
+    <row r="90" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>65</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="D90" t="s">
         <v>267</v>
       </c>
-      <c r="D90" t="s">
+      <c r="E90" t="s">
         <v>377</v>
       </c>
-      <c r="E90" t="s">
+      <c r="F90" t="s">
         <v>485</v>
       </c>
-      <c r="G90" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7">
+    </row>
+    <row r="91" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>31</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="D91" t="s">
         <v>268</v>
       </c>
-      <c r="D91" t="s">
+      <c r="E91" t="s">
         <v>378</v>
       </c>
-      <c r="E91" t="s">
+      <c r="F91" t="s">
         <v>486</v>
       </c>
-      <c r="G91" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7">
+    </row>
+    <row r="92" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>30</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D92" t="s">
         <v>269</v>
       </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
         <v>379</v>
       </c>
-      <c r="E92" t="s">
+      <c r="F92" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>30</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D93" t="s">
         <v>270</v>
       </c>
-      <c r="D93" t="s">
+      <c r="E93" t="s">
         <v>380</v>
       </c>
-      <c r="E93" t="s">
+      <c r="F93" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>30</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D94" t="s">
         <v>271</v>
       </c>
-      <c r="D94" t="s">
+      <c r="E94" t="s">
         <v>381</v>
       </c>
-      <c r="E94" t="s">
+      <c r="F94" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>66</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="D95" t="s">
         <v>272</v>
       </c>
-      <c r="D95" t="s">
+      <c r="E95" t="s">
         <v>382</v>
       </c>
-      <c r="E95" t="s">
+      <c r="F95" t="s">
         <v>490</v>
       </c>
-      <c r="G95" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7">
+    </row>
+    <row r="96" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>67</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="D96" t="s">
         <v>273</v>
       </c>
-      <c r="D96" t="s">
+      <c r="E96" t="s">
         <v>383</v>
       </c>
-      <c r="E96" t="s">
+      <c r="F96" t="s">
         <v>491</v>
       </c>
-      <c r="G96" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7">
-      <c r="B97" t="s">
+    </row>
+    <row r="97" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B97" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="D97" t="s">
         <v>274</v>
       </c>
-      <c r="D97" t="s">
+      <c r="E97" t="s">
         <v>384</v>
       </c>
-      <c r="E97" t="s">
+      <c r="F97" t="s">
         <v>492</v>
       </c>
-      <c r="G97" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7">
+    </row>
+    <row r="98" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>67</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="D98" t="s">
         <v>275</v>
       </c>
-      <c r="D98" t="s">
+      <c r="E98" t="s">
         <v>385</v>
       </c>
-      <c r="E98" t="s">
+      <c r="F98" t="s">
         <v>493</v>
       </c>
-      <c r="G98" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7">
+    </row>
+    <row r="99" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>67</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="D99" t="s">
         <v>276</v>
       </c>
-      <c r="D99" t="s">
+      <c r="E99" t="s">
         <v>386</v>
       </c>
-      <c r="E99" t="s">
+      <c r="F99" t="s">
         <v>494</v>
       </c>
-      <c r="G99" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7">
+    </row>
+    <row r="100" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>67</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="D100" t="s">
         <v>277</v>
       </c>
-      <c r="D100" t="s">
+      <c r="E100" t="s">
         <v>387</v>
       </c>
-      <c r="E100" t="s">
+      <c r="F100" t="s">
         <v>495</v>
       </c>
-      <c r="G100" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7">
+    </row>
+    <row r="101" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>23</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="D101" t="s">
         <v>278</v>
       </c>
-      <c r="D101" t="s">
+      <c r="E101" t="s">
         <v>388</v>
       </c>
-      <c r="E101" t="s">
+      <c r="F101" t="s">
         <v>496</v>
       </c>
-      <c r="G101" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7">
+    </row>
+    <row r="102" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>30</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B102" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D102" t="s">
         <v>279</v>
       </c>
-      <c r="D102" t="s">
+      <c r="E102" t="s">
         <v>389</v>
       </c>
-      <c r="E102" t="s">
+      <c r="F102" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>68</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C103" s="3" t="s">
+        <v>597</v>
+      </c>
+      <c r="D103" t="s">
         <v>280</v>
       </c>
-      <c r="D103" t="s">
+      <c r="E103" t="s">
         <v>390</v>
       </c>
-      <c r="E103" t="s">
+      <c r="F103" t="s">
         <v>498</v>
       </c>
-      <c r="G103" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7">
+    </row>
+    <row r="104" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>69</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B104" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C104" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="D104" t="s">
         <v>281</v>
       </c>
-      <c r="D104" t="s">
+      <c r="E104" t="s">
         <v>391</v>
       </c>
-      <c r="E104" t="s">
+      <c r="F104" t="s">
         <v>499</v>
       </c>
-      <c r="G104" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7">
+    </row>
+    <row r="105" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>69</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B105" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="D105" t="s">
         <v>282</v>
       </c>
-      <c r="D105" t="s">
+      <c r="E105" t="s">
         <v>392</v>
       </c>
-      <c r="E105" t="s">
+      <c r="F105" t="s">
         <v>500</v>
       </c>
-      <c r="G105" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7">
+    </row>
+    <row r="106" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>69</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D106" t="s">
         <v>283</v>
       </c>
-      <c r="D106" t="s">
+      <c r="E106" t="s">
         <v>393</v>
       </c>
-      <c r="E106" t="s">
+      <c r="F106" t="s">
         <v>501</v>
       </c>
-      <c r="G106" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7">
+    </row>
+    <row r="107" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>70</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C107" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="D107" t="s">
         <v>284</v>
       </c>
-      <c r="D107" t="s">
+      <c r="E107" t="s">
         <v>394</v>
       </c>
-      <c r="E107" t="s">
+      <c r="F107" t="s">
         <v>502</v>
       </c>
-      <c r="G107" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7">
+    </row>
+    <row r="108" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>69</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="D108" t="s">
         <v>285</v>
       </c>
-      <c r="D108" t="s">
+      <c r="E108" t="s">
         <v>395</v>
       </c>
-      <c r="E108" t="s">
+      <c r="F108" t="s">
         <v>503</v>
       </c>
-      <c r="G108" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7">
+    </row>
+    <row r="109" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>67</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="D109" t="s">
         <v>286</v>
       </c>
-      <c r="D109" t="s">
+      <c r="E109" t="s">
         <v>396</v>
       </c>
-      <c r="E109" t="s">
+      <c r="F109" t="s">
         <v>504</v>
       </c>
-      <c r="G109" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7">
+    </row>
+    <row r="110" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>71</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="D110" t="s">
         <v>287</v>
       </c>
-      <c r="D110" t="s">
+      <c r="E110" t="s">
         <v>397</v>
       </c>
-      <c r="E110" t="s">
+      <c r="F110" t="s">
         <v>505</v>
       </c>
-      <c r="G110" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7">
+    </row>
+    <row r="111" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>31</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="C111" t="s">
+      <c r="D111" t="s">
         <v>288</v>
       </c>
-      <c r="D111" t="s">
+      <c r="E111" t="s">
         <v>398</v>
       </c>
-      <c r="E111" t="s">
+      <c r="F111" t="s">
         <v>506</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE2933C-316C-4C86-BD83-070D2666521A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>